<commit_message>
add a2c and cleaning and fix altitude
</commit_message>
<xml_diff>
--- a/controller.xlsx
+++ b/controller.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\azadi tez\tez\azadi\RL-for-control-quad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="learn" sheetId="1" r:id="rId1"/>
     <sheet name="run" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>environment name</t>
   </si>
@@ -28,6 +23,15 @@
     <t>iter number</t>
   </si>
   <si>
+    <t>path_planning</t>
+  </si>
+  <si>
+    <t>attitude_test</t>
+  </si>
+  <si>
+    <t>altitude_test</t>
+  </si>
+  <si>
     <t>attitude_discrete</t>
   </si>
   <si>
@@ -37,10 +41,31 @@
     <t>attitude_fragment</t>
   </si>
   <si>
-    <t>attitude_test</t>
-  </si>
-  <si>
-    <t>path_planning</t>
+    <t>altitude_discrete</t>
+  </si>
+  <si>
+    <t>altitude_continuous</t>
+  </si>
+  <si>
+    <t>altitude_fragment</t>
+  </si>
+  <si>
+    <t>attitude_discrete_a2c</t>
+  </si>
+  <si>
+    <t>attitude_continuous_A2C</t>
+  </si>
+  <si>
+    <t>attitude_fragment_A2C</t>
+  </si>
+  <si>
+    <t>altitude_discrete_A2C</t>
+  </si>
+  <si>
+    <t>altitude_continuous_A2C</t>
+  </si>
+  <si>
+    <t>altitude_fragment_A2C</t>
   </si>
   <si>
     <t>run</t>
@@ -49,8 +74,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,14 +138,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -167,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,10 +216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,7 +250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -410,16 +425,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -435,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -443,7 +456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -451,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -459,12 +472,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>250</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -473,22 +566,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -496,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -504,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -512,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -520,12 +613,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>